<commit_message>
changed field from Folder to Functional Area
</commit_message>
<xml_diff>
--- a/template_new.xlsx
+++ b/template_new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="39420" yWindow="-3060" windowWidth="25360" windowHeight="16460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
-    <t>Folder</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
   </si>
   <si>
     <t>Jira Ticket</t>
+  </si>
+  <si>
+    <t>Functional Area</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -458,63 +458,63 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="30">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated necessary column header names
</commit_message>
<xml_diff>
--- a/template_new.xlsx
+++ b/template_new.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -73,7 +73,7 @@
     <t>Jira Ticket</t>
   </si>
   <si>
-    <t>Functional Area</t>
+    <t>Section</t>
   </si>
 </sst>
 </file>

</xml_diff>